<commit_message>
Update the Reports Testing Folder
</commit_message>
<xml_diff>
--- a/CSci 136 - 05 Test Case Management (Sample).xlsx
+++ b/CSci 136 - 05 Test Case Management (Sample).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Documents\VSU\DCST\BS Computer Science\3rd Year_2024-2025\2nd Semester\CSci 136_Software Engineering 2\Laboratory\LAB 8\MachuPicchuTCM-main - test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Documents\VSU\DCST\BS Computer Science\3rd Year_2024-2025\2nd Semester\CSci 136_Software Engineering 2\Laboratory\LAB 8\MachuPicchuTCM-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02A8682-323F-433E-8B2C-29E3EA489C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AFA0C4-CC76-4DA7-9165-DB7416D248A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="622">
   <si>
     <t>Test Cases</t>
   </si>
@@ -1878,6 +1878,15 @@
   </si>
   <si>
     <t xml:space="preserve">      Auth testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Transaction Reports testing - Add</t>
+  </si>
+  <si>
+    <t>REP-0008</t>
+  </si>
+  <si>
+    <t>Verify that transaction is saved successfully.</t>
   </si>
 </sst>
 </file>
@@ -2255,10 +2264,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C124"/>
+  <dimension ref="A1:C123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2657,203 +2666,203 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="13.2">
-      <c r="A38" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A38" s="15" t="s">
+        <v>601</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" ht="13.2">
-      <c r="A39" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>84</v>
+      <c r="A39" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>606</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="13.2">
-      <c r="A40" s="15" t="s">
-        <v>601</v>
+      <c r="A40" s="2" t="s">
+        <v>568</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" ht="13.2">
-      <c r="A41" s="14" t="s">
-        <v>602</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>606</v>
+      <c r="A41" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="13.2">
-      <c r="A42" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="18.600000000000001" customHeight="1">
+      <c r="A42" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="13.2">
       <c r="A43" s="4" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="18.600000000000001" customHeight="1">
-      <c r="A44" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="13.2">
+      <c r="A44" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
     </row>
     <row r="45" spans="1:3" ht="13.2">
-      <c r="A45" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="13.2">
-      <c r="A46" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="A45" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="9"/>
+    </row>
+    <row r="46" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A46" s="14" t="s">
+        <v>619</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>621</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="13.2">
-      <c r="A47" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="9"/>
+      <c r="A47" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="13.2">
-      <c r="A48" s="4" t="s">
-        <v>214</v>
+      <c r="A48" s="14" t="s">
+        <v>603</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>26</v>
+        <v>231</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>604</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="13.2">
       <c r="A49" s="14" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>604</v>
+        <v>566</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="13.2">
-      <c r="A50" s="14" t="s">
-        <v>605</v>
+      <c r="A50" s="4" t="s">
+        <v>219</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>231</v>
+        <v>607</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>80</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="13.2">
       <c r="A51" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>566</v>
+        <v>608</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="13.2">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>221</v>
+        <v>615</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1">
-      <c r="A53" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="C53" s="6" t="s">
         <v>224</v>
       </c>
     </row>
+    <row r="53" spans="1:3" ht="13.2">
+      <c r="A53" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="9"/>
+    </row>
     <row r="54" spans="1:3" ht="13.2">
-      <c r="A54" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B54" s="8"/>
-      <c r="C54" s="9"/>
+      <c r="A54" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="B54" s="17" t="s">
+        <v>620</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>610</v>
+      </c>
     </row>
     <row r="55" spans="1:3" ht="13.2">
-      <c r="A55" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>609</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>610</v>
-      </c>
+      <c r="A55" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
     </row>
     <row r="56" spans="1:3" ht="13.2">
-      <c r="A56" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
+      <c r="A56" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B56" s="8"/>
+      <c r="C56" s="9"/>
     </row>
     <row r="57" spans="1:3" ht="13.2">
-      <c r="A57" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="9"/>
+      <c r="A57" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="58" spans="1:3" ht="13.2">
-      <c r="A58" s="4" t="s">
-        <v>321</v>
+      <c r="A58" s="18" t="s">
+        <v>324</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>323</v>
@@ -2861,10 +2870,10 @@
     </row>
     <row r="59" spans="1:3" ht="13.2">
       <c r="A59" s="18" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>323</v>
@@ -2872,10 +2881,10 @@
     </row>
     <row r="60" spans="1:3" ht="13.2">
       <c r="A60" s="18" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>323</v>
@@ -2883,10 +2892,10 @@
     </row>
     <row r="61" spans="1:3" ht="13.2">
       <c r="A61" s="18" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>323</v>
@@ -2894,10 +2903,10 @@
     </row>
     <row r="62" spans="1:3" ht="13.2">
       <c r="A62" s="18" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>323</v>
@@ -2905,21 +2914,21 @@
     </row>
     <row r="63" spans="1:3" ht="13.2">
       <c r="A63" s="18" t="s">
-        <v>332</v>
+        <v>570</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="13.2">
-      <c r="A64" s="18" t="s">
-        <v>570</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>335</v>
+      <c r="A64" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>337</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>323</v>
@@ -2927,39 +2936,39 @@
     </row>
     <row r="65" spans="1:3" ht="13.2">
       <c r="A65" s="19" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B65" s="17" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="13.2">
-      <c r="A66" s="19" t="s">
-        <v>613</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>323</v>
-      </c>
+      <c r="A66" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B66" s="8"/>
+      <c r="C66" s="9"/>
     </row>
     <row r="67" spans="1:3" ht="13.2">
-      <c r="A67" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B67" s="8"/>
-      <c r="C67" s="9"/>
+      <c r="A67" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="68" spans="1:3" ht="13.2">
-      <c r="A68" s="4" t="s">
-        <v>321</v>
+      <c r="A68" s="18" t="s">
+        <v>324</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C68" s="18" t="s">
         <v>350</v>
@@ -2967,10 +2976,10 @@
     </row>
     <row r="69" spans="1:3" ht="13.2">
       <c r="A69" s="18" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>350</v>
@@ -2978,10 +2987,10 @@
     </row>
     <row r="70" spans="1:3" ht="13.2">
       <c r="A70" s="18" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C70" s="18" t="s">
         <v>350</v>
@@ -2989,10 +2998,10 @@
     </row>
     <row r="71" spans="1:3" ht="13.2">
       <c r="A71" s="18" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C71" s="18" t="s">
         <v>350</v>
@@ -3000,10 +3009,10 @@
     </row>
     <row r="72" spans="1:3" ht="13.2">
       <c r="A72" s="18" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>350</v>
@@ -3011,304 +3020,304 @@
     </row>
     <row r="73" spans="1:3" ht="13.2">
       <c r="A73" s="18" t="s">
-        <v>332</v>
+        <v>570</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="13.2">
-      <c r="A74" s="18" t="s">
-        <v>570</v>
+      <c r="A74" s="19" t="s">
+        <v>614</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C74" s="18" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="13.2">
-      <c r="A75" s="19" t="s">
-        <v>614</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="C75" s="18" t="s">
-        <v>350</v>
-      </c>
+      <c r="A75" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B75" s="8"/>
+      <c r="C75" s="9"/>
     </row>
     <row r="76" spans="1:3" ht="13.2">
-      <c r="A76" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="B76" s="8"/>
-      <c r="C76" s="9"/>
+      <c r="A76" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="77" spans="1:3" ht="13.2">
       <c r="A77" s="18" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="B77" s="17" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C77" s="18" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="13.2">
       <c r="A78" s="18" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="13.2">
-      <c r="A79" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="B79" s="17" t="s">
-        <v>356</v>
-      </c>
-      <c r="C79" s="18" t="s">
-        <v>378</v>
-      </c>
+      <c r="A79" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B79" s="8"/>
+      <c r="C79" s="9"/>
     </row>
     <row r="80" spans="1:3" ht="13.2">
-      <c r="A80" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="B80" s="8"/>
-      <c r="C80" s="9"/>
+      <c r="A80" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="B80" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="81" spans="1:3" ht="13.2">
       <c r="A81" s="18" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="13.2">
       <c r="A82" s="18" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C82" s="18" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="13.2">
-      <c r="A83" s="18" t="s">
-        <v>389</v>
-      </c>
-      <c r="B83" s="17" t="s">
-        <v>359</v>
-      </c>
-      <c r="C83" s="18" t="s">
-        <v>391</v>
-      </c>
+      <c r="A83" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B83" s="3"/>
+      <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:3" ht="13.2">
-      <c r="A84" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
+      <c r="A84" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="9"/>
     </row>
     <row r="85" spans="1:3" ht="13.2">
-      <c r="A85" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="B85" s="8"/>
-      <c r="C85" s="9"/>
+      <c r="A85" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="13.2">
       <c r="A86" s="4" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="C86" s="12" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="13.2">
       <c r="A87" s="4" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="13.2">
       <c r="A88" s="4" t="s">
-        <v>400</v>
+        <v>616</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="13.2">
       <c r="A89" s="4" t="s">
-        <v>616</v>
+        <v>406</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="13.2">
-      <c r="A90" s="4" t="s">
-        <v>406</v>
+      <c r="A90" s="14" t="s">
+        <v>409</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="13.2">
-      <c r="A91" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="C91" s="12" t="s">
-        <v>411</v>
-      </c>
+      <c r="A91" s="13" t="s">
+        <v>571</v>
+      </c>
+      <c r="B91" s="8"/>
+      <c r="C91" s="9"/>
     </row>
     <row r="92" spans="1:3" ht="13.2">
-      <c r="A92" s="13" t="s">
-        <v>571</v>
-      </c>
-      <c r="B92" s="8"/>
-      <c r="C92" s="9"/>
+      <c r="A92" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>416</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>576</v>
+      </c>
     </row>
     <row r="93" spans="1:3" ht="13.2">
       <c r="A93" s="4" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="13.2">
       <c r="A94" s="4" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="13.2">
       <c r="A95" s="4" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="13.2">
       <c r="A96" s="4" t="s">
-        <v>575</v>
+        <v>581</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C96" s="12" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="13.2">
-      <c r="A97" s="4" t="s">
-        <v>581</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="C97" s="12" t="s">
-        <v>580</v>
-      </c>
+      <c r="A97" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
     </row>
     <row r="98" spans="1:3" ht="13.2">
-      <c r="A98" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
+      <c r="A98" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B98" s="8"/>
+      <c r="C98" s="9"/>
     </row>
     <row r="99" spans="1:3" ht="13.2">
-      <c r="A99" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="B99" s="8"/>
-      <c r="C99" s="9"/>
+      <c r="A99" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="100" spans="1:3" ht="13.2">
-      <c r="A100" s="4" t="s">
-        <v>617</v>
-      </c>
-      <c r="B100" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="C100" s="6" t="s">
-        <v>437</v>
-      </c>
+      <c r="A100" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="B100" s="8"/>
+      <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" ht="13.2">
       <c r="A101" s="7" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B101" s="8"/>
       <c r="C101" s="9"/>
     </row>
     <row r="102" spans="1:3" ht="13.2">
-      <c r="A102" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="B102" s="8"/>
-      <c r="C102" s="9"/>
+      <c r="A102" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B102" s="17" t="s">
+        <v>436</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="103" spans="1:3" ht="13.2">
-      <c r="A103" s="4" t="s">
-        <v>464</v>
+      <c r="A103" s="18" t="s">
+        <v>467</v>
       </c>
       <c r="B103" s="17" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>466</v>
@@ -3316,10 +3325,10 @@
     </row>
     <row r="104" spans="1:3" ht="13.2">
       <c r="A104" s="18" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="B104" s="17" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>466</v>
@@ -3327,10 +3336,10 @@
     </row>
     <row r="105" spans="1:3" ht="13.2">
       <c r="A105" s="18" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B105" s="17" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>466</v>
@@ -3338,21 +3347,21 @@
     </row>
     <row r="106" spans="1:3" ht="13.2">
       <c r="A106" s="18" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="13.2">
-      <c r="A107" s="18" t="s">
-        <v>473</v>
+      <c r="A107" s="19" t="s">
+        <v>611</v>
       </c>
       <c r="B107" s="17" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>466</v>
@@ -3360,50 +3369,50 @@
     </row>
     <row r="108" spans="1:3" ht="13.2">
       <c r="A108" s="19" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="13.2">
-      <c r="A109" s="19" t="s">
-        <v>612</v>
+      <c r="A109" s="18" t="s">
+        <v>475</v>
       </c>
       <c r="B109" s="17" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="13.2">
-      <c r="A110" s="18" t="s">
-        <v>475</v>
-      </c>
-      <c r="B110" s="17" t="s">
-        <v>457</v>
-      </c>
-      <c r="C110" s="6" t="s">
+      <c r="A110" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="B110" s="8"/>
+      <c r="C110" s="9"/>
+    </row>
+    <row r="111" spans="1:3" ht="13.2">
+      <c r="A111" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B111" s="17" t="s">
+        <v>460</v>
+      </c>
+      <c r="C111" s="6" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" ht="13.2">
-      <c r="A111" s="7" t="s">
-        <v>489</v>
-      </c>
-      <c r="B111" s="8"/>
-      <c r="C111" s="9"/>
     </row>
     <row r="112" spans="1:3" ht="13.2">
       <c r="A112" s="4" t="s">
-        <v>464</v>
+        <v>618</v>
       </c>
       <c r="B112" s="17" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="C112" s="6" t="s">
         <v>466</v>
@@ -3411,10 +3420,10 @@
     </row>
     <row r="113" spans="1:3" ht="13.2">
       <c r="A113" s="4" t="s">
-        <v>618</v>
+        <v>469</v>
       </c>
       <c r="B113" s="17" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>466</v>
@@ -3422,10 +3431,10 @@
     </row>
     <row r="114" spans="1:3" ht="13.2">
       <c r="A114" s="4" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B114" s="17" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>466</v>
@@ -3433,21 +3442,21 @@
     </row>
     <row r="115" spans="1:3" ht="13.2">
       <c r="A115" s="4" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="13.2">
-      <c r="A116" s="4" t="s">
-        <v>473</v>
+      <c r="A116" s="19" t="s">
+        <v>611</v>
       </c>
       <c r="B116" s="17" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>466</v>
@@ -3455,21 +3464,21 @@
     </row>
     <row r="117" spans="1:3" ht="13.2">
       <c r="A117" s="19" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B117" s="17" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="13.2">
-      <c r="A118" s="19" t="s">
-        <v>612</v>
+      <c r="A118" s="4" t="s">
+        <v>475</v>
       </c>
       <c r="B118" s="17" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>466</v>
@@ -3477,63 +3486,52 @@
     </row>
     <row r="119" spans="1:3" ht="13.2">
       <c r="A119" s="4" t="s">
-        <v>475</v>
+        <v>502</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>466</v>
+        <v>504</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="13.2">
-      <c r="A120" s="4" t="s">
-        <v>502</v>
-      </c>
-      <c r="B120" s="17" t="s">
-        <v>480</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>504</v>
-      </c>
+      <c r="A120" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
     </row>
     <row r="121" spans="1:3" ht="13.2">
-      <c r="A121" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
+      <c r="A121" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="122" spans="1:3" ht="13.2">
       <c r="A122" s="4" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="13.2">
       <c r="A123" s="4" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="13.2">
-      <c r="A124" s="4" t="s">
-        <v>524</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="C124" s="6" t="s">
         <v>526</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update CUSTOMER and added Authentication Test Suite and Case.
</commit_message>
<xml_diff>
--- a/CSci 136 - 05 Test Case Management (Sample).xlsx
+++ b/CSci 136 - 05 Test Case Management (Sample).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Documents\VSU\DCST\BS Computer Science\3rd Year_2024-2025\2nd Semester\CSci 136_Software Engineering 2\Laboratory\LAB 8\MachuPicchuTCM-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AFA0C4-CC76-4DA7-9165-DB7416D248A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CE1CE5-F4E8-4692-943C-985CD677A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="626">
   <si>
     <t>Test Cases</t>
   </si>
@@ -1887,6 +1887,18 @@
   </si>
   <si>
     <t>Verify that transaction is saved successfully.</t>
+  </si>
+  <si>
+    <t>Authentication Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Authentication Testing - Log-in</t>
+  </si>
+  <si>
+    <t>AUTH-0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user can log-in successfully. </t>
   </si>
 </sst>
 </file>
@@ -1945,7 +1957,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1962,6 +1974,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1992,7 +2016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2045,6 +2069,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2264,10 +2298,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C123"/>
+  <dimension ref="A1:C125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -2291,50 +2325,46 @@
     </row>
     <row r="2" spans="1:3" ht="13.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>622</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="13.2">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
+    <row r="3" spans="1:3" s="20" customFormat="1" ht="13.2">
+      <c r="A3" s="21" t="s">
+        <v>623</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>624</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.2">
-      <c r="A4" s="4" t="s">
-        <v>562</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="13.2">
       <c r="A5" s="4" t="s">
-        <v>563</v>
+        <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>564</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.2">
       <c r="A6" s="4" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>9</v>
@@ -2342,538 +2372,538 @@
     </row>
     <row r="7" spans="1:3" ht="13.2">
       <c r="A7" s="4" t="s">
-        <v>12</v>
+        <v>563</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>14</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="13.2">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>567</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.2">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="13.2">
-      <c r="A10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="13.2">
       <c r="A11" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>36</v>
+        <v>22</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="13.2">
-      <c r="A12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>39</v>
-      </c>
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" ht="13.2">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="13.2">
       <c r="A14" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.2">
       <c r="A15" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="13.2">
       <c r="A16" s="4" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="13.2">
       <c r="A17" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="13.2">
-      <c r="A18" s="15" t="s">
-        <v>582</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="13.2">
       <c r="A19" s="4" t="s">
-        <v>583</v>
+        <v>50</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>594</v>
+        <v>51</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>590</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="13.2">
-      <c r="A20" s="4" t="s">
-        <v>584</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>595</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>591</v>
-      </c>
+      <c r="A20" s="15" t="s">
+        <v>582</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" ht="13.2">
       <c r="A21" s="4" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="13.2">
       <c r="A22" s="4" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="13.2">
       <c r="A23" s="4" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>26</v>
+        <v>592</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="13.2">
       <c r="A24" s="4" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>29</v>
+        <v>593</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="13.2">
       <c r="A25" s="4" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="13.2">
-      <c r="A26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="A26" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>599</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="13.2">
       <c r="A27" s="4" t="s">
-        <v>53</v>
+        <v>589</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>54</v>
+        <v>600</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="13.2">
-      <c r="A28" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="A28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" ht="13.2">
       <c r="A29" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="13.2">
       <c r="A30" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="13.2">
       <c r="A31" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="13.2">
       <c r="A32" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="13.2">
       <c r="A33" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="13.2">
-      <c r="A34" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="A34" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="13.2">
       <c r="A35" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="13.2">
-      <c r="A36" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="A36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" ht="13.2">
       <c r="A37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="13.2">
+      <c r="A38" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="13.2">
+      <c r="A39" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="13.2">
-      <c r="A38" s="15" t="s">
+    <row r="40" spans="1:3" ht="13.2">
+      <c r="A40" s="15" t="s">
         <v>601</v>
-      </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="1:3" ht="13.2">
-      <c r="A39" s="14" t="s">
-        <v>602</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>606</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="13.2">
-      <c r="A40" s="2" t="s">
-        <v>568</v>
       </c>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" ht="13.2">
-      <c r="A41" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>89</v>
+      <c r="A41" s="14" t="s">
+        <v>602</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>606</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="18.600000000000001" customHeight="1">
-      <c r="A42" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>29</v>
-      </c>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="13.2">
+      <c r="A42" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" ht="13.2">
       <c r="A43" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="18.600000000000001" customHeight="1">
+      <c r="A44" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="13.2">
+      <c r="A45" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B45" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="13.2">
-      <c r="A44" s="2" t="s">
+    <row r="46" spans="1:3" ht="13.2">
+      <c r="A46" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="1:3" ht="13.2">
-      <c r="A45" s="7" t="s">
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" ht="13.2">
+      <c r="A47" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="9"/>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A46" s="14" t="s">
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
+    </row>
+    <row r="48" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A48" s="14" t="s">
         <v>619</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B48" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C48" s="16" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="13.2">
-      <c r="A47" s="4" t="s">
+    <row r="49" spans="1:3" ht="13.2">
+      <c r="A49" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="13.2">
-      <c r="A48" s="14" t="s">
+    <row r="50" spans="1:3" ht="13.2">
+      <c r="A50" s="14" t="s">
         <v>603</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B50" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C50" s="16" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="13.2">
-      <c r="A49" s="14" t="s">
+    <row r="51" spans="1:3" ht="13.2">
+      <c r="A51" s="14" t="s">
         <v>605</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B51" s="5" t="s">
         <v>566</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13.2">
-      <c r="A50" s="4" t="s">
+    <row r="52" spans="1:3" ht="13.2">
+      <c r="A52" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B52" s="5" t="s">
         <v>607</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C52" s="6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="13.2">
-      <c r="A51" s="4" t="s">
+    <row r="53" spans="1:3" ht="13.2">
+      <c r="A53" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B53" s="5" t="s">
         <v>608</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C53" s="6" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1">
-      <c r="A52" s="4" t="s">
+    <row r="54" spans="1:3" ht="15" customHeight="1">
+      <c r="A54" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B54" s="5" t="s">
         <v>609</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="13.2">
-      <c r="A53" s="7" t="s">
+    <row r="55" spans="1:3" ht="13.2">
+      <c r="A55" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="B53" s="8"/>
-      <c r="C53" s="9"/>
-    </row>
-    <row r="54" spans="1:3" ht="13.2">
-      <c r="A54" s="4" t="s">
+      <c r="B55" s="8"/>
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="1:3" ht="13.2">
+      <c r="A56" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B56" s="17" t="s">
         <v>620</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C56" s="16" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="13.2">
-      <c r="A55" s="2" t="s">
+    <row r="57" spans="1:3" ht="13.2">
+      <c r="A57" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-    </row>
-    <row r="56" spans="1:3" ht="13.2">
-      <c r="A56" s="7" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" ht="13.2">
+      <c r="A58" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="9"/>
-    </row>
-    <row r="57" spans="1:3" ht="13.2">
-      <c r="A57" s="4" t="s">
+      <c r="B58" s="8"/>
+      <c r="C58" s="9"/>
+    </row>
+    <row r="59" spans="1:3" ht="13.2">
+      <c r="A59" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B59" s="5" t="s">
         <v>322</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="13.2">
-      <c r="A58" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="13.2">
-      <c r="A59" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>327</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>323</v>
@@ -2881,10 +2911,10 @@
     </row>
     <row r="60" spans="1:3" ht="13.2">
       <c r="A60" s="18" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>323</v>
@@ -2892,10 +2922,10 @@
     </row>
     <row r="61" spans="1:3" ht="13.2">
       <c r="A61" s="18" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>323</v>
@@ -2903,10 +2933,10 @@
     </row>
     <row r="62" spans="1:3" ht="13.2">
       <c r="A62" s="18" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>323</v>
@@ -2914,72 +2944,72 @@
     </row>
     <row r="63" spans="1:3" ht="13.2">
       <c r="A63" s="18" t="s">
-        <v>570</v>
+        <v>330</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="13.2">
-      <c r="A64" s="19" t="s">
-        <v>614</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>337</v>
+      <c r="A64" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>333</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="13.2">
-      <c r="A65" s="19" t="s">
-        <v>613</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>339</v>
+      <c r="A65" s="18" t="s">
+        <v>570</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>335</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="13.2">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="13.2">
+      <c r="A67" s="19" t="s">
+        <v>613</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="13.2">
+      <c r="A68" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="B66" s="8"/>
-      <c r="C66" s="9"/>
-    </row>
-    <row r="67" spans="1:3" ht="13.2">
-      <c r="A67" s="4" t="s">
+      <c r="B68" s="8"/>
+      <c r="C68" s="9"/>
+    </row>
+    <row r="69" spans="1:3" ht="13.2">
+      <c r="A69" s="4" t="s">
         <v>321</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B69" s="17" t="s">
         <v>341</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="13.2">
-      <c r="A68" s="18" t="s">
-        <v>324</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>343</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="13.2">
-      <c r="A69" s="18" t="s">
-        <v>326</v>
-      </c>
-      <c r="B69" s="17" t="s">
-        <v>345</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>350</v>
@@ -2987,10 +3017,10 @@
     </row>
     <row r="70" spans="1:3" ht="13.2">
       <c r="A70" s="18" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C70" s="18" t="s">
         <v>350</v>
@@ -2998,10 +3028,10 @@
     </row>
     <row r="71" spans="1:3" ht="13.2">
       <c r="A71" s="18" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C71" s="18" t="s">
         <v>350</v>
@@ -3009,10 +3039,10 @@
     </row>
     <row r="72" spans="1:3" ht="13.2">
       <c r="A72" s="18" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>350</v>
@@ -3020,315 +3050,315 @@
     </row>
     <row r="73" spans="1:3" ht="13.2">
       <c r="A73" s="18" t="s">
-        <v>570</v>
+        <v>330</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="13.2">
-      <c r="A74" s="19" t="s">
-        <v>614</v>
+      <c r="A74" s="18" t="s">
+        <v>332</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C74" s="18" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="13.2">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="18" t="s">
+        <v>570</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="13.2">
+      <c r="A76" s="19" t="s">
+        <v>614</v>
+      </c>
+      <c r="B76" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="13.2">
+      <c r="A77" s="7" t="s">
         <v>363</v>
       </c>
-      <c r="B75" s="8"/>
-      <c r="C75" s="9"/>
-    </row>
-    <row r="76" spans="1:3" ht="13.2">
-      <c r="A76" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="13.2">
-      <c r="A77" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>355</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>375</v>
-      </c>
+      <c r="B77" s="8"/>
+      <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3" ht="13.2">
       <c r="A78" s="18" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="13.2">
-      <c r="A79" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="B79" s="8"/>
-      <c r="C79" s="9"/>
+      <c r="A79" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="B79" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="80" spans="1:3" ht="13.2">
       <c r="A80" s="18" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="13.2">
-      <c r="A81" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>358</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>388</v>
-      </c>
+      <c r="A81" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="B81" s="8"/>
+      <c r="C81" s="9"/>
     </row>
     <row r="82" spans="1:3" ht="13.2">
       <c r="A82" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="B82" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="13.2">
+      <c r="A83" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="B83" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="13.2">
+      <c r="A84" s="18" t="s">
         <v>389</v>
       </c>
-      <c r="B82" s="17" t="s">
+      <c r="B84" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="C84" s="18" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="13.2">
-      <c r="A83" s="2" t="s">
+    <row r="85" spans="1:3" ht="13.2">
+      <c r="A85" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B83" s="3"/>
-      <c r="C83" s="3"/>
-    </row>
-    <row r="84" spans="1:3" ht="13.2">
-      <c r="A84" s="13" t="s">
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+    </row>
+    <row r="86" spans="1:3" ht="13.2">
+      <c r="A86" s="13" t="s">
         <v>393</v>
       </c>
-      <c r="B84" s="8"/>
-      <c r="C84" s="9"/>
-    </row>
-    <row r="85" spans="1:3" ht="13.2">
-      <c r="A85" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="C85" s="12" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="13.2">
-      <c r="A86" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="C86" s="12" t="s">
-        <v>399</v>
-      </c>
+      <c r="B86" s="8"/>
+      <c r="C86" s="9"/>
     </row>
     <row r="87" spans="1:3" ht="13.2">
       <c r="A87" s="4" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="13.2">
       <c r="A88" s="4" t="s">
-        <v>616</v>
+        <v>397</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="13.2">
       <c r="A89" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="13.2">
+      <c r="A90" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="B90" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="13.2">
+      <c r="A91" s="4" t="s">
         <v>406</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B91" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="C89" s="12" t="s">
+      <c r="C91" s="12" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="13.2">
-      <c r="A90" s="14" t="s">
+    <row r="92" spans="1:3" ht="13.2">
+      <c r="A92" s="14" t="s">
         <v>409</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B92" s="5" t="s">
         <v>410</v>
       </c>
-      <c r="C90" s="12" t="s">
+      <c r="C92" s="12" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="13.2">
-      <c r="A91" s="13" t="s">
+    <row r="93" spans="1:3" ht="13.2">
+      <c r="A93" s="13" t="s">
         <v>571</v>
       </c>
-      <c r="B91" s="8"/>
-      <c r="C91" s="9"/>
-    </row>
-    <row r="92" spans="1:3" ht="13.2">
-      <c r="A92" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="C92" s="12" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="13.2">
-      <c r="A93" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="C93" s="12" t="s">
-        <v>577</v>
-      </c>
+      <c r="B93" s="8"/>
+      <c r="C93" s="9"/>
     </row>
     <row r="94" spans="1:3" ht="13.2">
       <c r="A94" s="4" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="13.2">
       <c r="A95" s="4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="C95" s="12" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="13.2">
       <c r="A96" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="13.2">
+      <c r="A97" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="13.2">
+      <c r="A98" s="4" t="s">
         <v>581</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B98" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="C96" s="12" t="s">
+      <c r="C98" s="12" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="13.2">
-      <c r="A97" s="2" t="s">
+    <row r="99" spans="1:3" ht="13.2">
+      <c r="A99" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-    </row>
-    <row r="98" spans="1:3" ht="13.2">
-      <c r="A98" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="B98" s="8"/>
-      <c r="C98" s="9"/>
-    </row>
-    <row r="99" spans="1:3" ht="13.2">
-      <c r="A99" s="4" t="s">
-        <v>617</v>
-      </c>
-      <c r="B99" s="5" t="s">
-        <v>433</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>437</v>
-      </c>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
     </row>
     <row r="100" spans="1:3" ht="13.2">
       <c r="A100" s="7" t="s">
-        <v>462</v>
+        <v>431</v>
       </c>
       <c r="B100" s="8"/>
       <c r="C100" s="9"/>
     </row>
     <row r="101" spans="1:3" ht="13.2">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="13.2">
+      <c r="A102" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="B102" s="8"/>
+      <c r="C102" s="9"/>
+    </row>
+    <row r="103" spans="1:3" ht="13.2">
+      <c r="A103" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="B101" s="8"/>
-      <c r="C101" s="9"/>
-    </row>
-    <row r="102" spans="1:3" ht="13.2">
-      <c r="A102" s="4" t="s">
+      <c r="B103" s="8"/>
+      <c r="C103" s="9"/>
+    </row>
+    <row r="104" spans="1:3" ht="13.2">
+      <c r="A104" s="4" t="s">
         <v>464</v>
       </c>
-      <c r="B102" s="17" t="s">
+      <c r="B104" s="17" t="s">
         <v>436</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="13.2">
-      <c r="A103" s="18" t="s">
-        <v>467</v>
-      </c>
-      <c r="B103" s="17" t="s">
-        <v>439</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="13.2">
-      <c r="A104" s="18" t="s">
-        <v>469</v>
-      </c>
-      <c r="B104" s="17" t="s">
-        <v>442</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>466</v>
@@ -3336,10 +3366,10 @@
     </row>
     <row r="105" spans="1:3" ht="13.2">
       <c r="A105" s="18" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B105" s="17" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>466</v>
@@ -3347,83 +3377,83 @@
     </row>
     <row r="106" spans="1:3" ht="13.2">
       <c r="A106" s="18" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="13.2">
-      <c r="A107" s="19" t="s">
-        <v>611</v>
+      <c r="A107" s="18" t="s">
+        <v>471</v>
       </c>
       <c r="B107" s="17" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="13.2">
-      <c r="A108" s="19" t="s">
-        <v>612</v>
+      <c r="A108" s="18" t="s">
+        <v>473</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="13.2">
-      <c r="A109" s="18" t="s">
-        <v>475</v>
+      <c r="A109" s="19" t="s">
+        <v>611</v>
       </c>
       <c r="B109" s="17" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="13.2">
-      <c r="A110" s="7" t="s">
-        <v>489</v>
-      </c>
-      <c r="B110" s="8"/>
-      <c r="C110" s="9"/>
+      <c r="A110" s="19" t="s">
+        <v>612</v>
+      </c>
+      <c r="B110" s="17" t="s">
+        <v>454</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="111" spans="1:3" ht="13.2">
-      <c r="A111" s="4" t="s">
-        <v>464</v>
+      <c r="A111" s="18" t="s">
+        <v>475</v>
       </c>
       <c r="B111" s="17" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="13.2">
-      <c r="A112" s="4" t="s">
-        <v>618</v>
-      </c>
-      <c r="B112" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>466</v>
-      </c>
+      <c r="A112" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="B112" s="8"/>
+      <c r="C112" s="9"/>
     </row>
     <row r="113" spans="1:3" ht="13.2">
       <c r="A113" s="4" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B113" s="17" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>466</v>
@@ -3431,10 +3461,10 @@
     </row>
     <row r="114" spans="1:3" ht="13.2">
       <c r="A114" s="4" t="s">
-        <v>471</v>
+        <v>618</v>
       </c>
       <c r="B114" s="17" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>466</v>
@@ -3442,96 +3472,118 @@
     </row>
     <row r="115" spans="1:3" ht="13.2">
       <c r="A115" s="4" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="13.2">
-      <c r="A116" s="19" t="s">
-        <v>611</v>
+      <c r="A116" s="4" t="s">
+        <v>471</v>
       </c>
       <c r="B116" s="17" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="13.2">
-      <c r="A117" s="19" t="s">
-        <v>612</v>
+      <c r="A117" s="4" t="s">
+        <v>473</v>
       </c>
       <c r="B117" s="17" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C117" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="13.2">
-      <c r="A118" s="4" t="s">
-        <v>475</v>
+      <c r="A118" s="19" t="s">
+        <v>611</v>
       </c>
       <c r="B118" s="17" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="13.2">
-      <c r="A119" s="4" t="s">
-        <v>502</v>
+      <c r="A119" s="19" t="s">
+        <v>612</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>504</v>
+        <v>466</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="13.2">
-      <c r="A120" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
+      <c r="A120" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="B120" s="17" t="s">
+        <v>478</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="121" spans="1:3" ht="13.2">
       <c r="A121" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>510</v>
+        <v>502</v>
+      </c>
+      <c r="B121" s="17" t="s">
+        <v>480</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>520</v>
+        <v>504</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="13.2">
-      <c r="A122" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>523</v>
-      </c>
+      <c r="A122" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
     </row>
     <row r="123" spans="1:3" ht="13.2">
       <c r="A123" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="13.2">
+      <c r="A124" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="13.2">
+      <c r="A125" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="B125" s="5" t="s">
         <v>516</v>
       </c>
-      <c r="C123" s="6" t="s">
+      <c r="C125" s="6" t="s">
         <v>526</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Category and Supplier test cases
</commit_message>
<xml_diff>
--- a/CSci 136 - 05 Test Case Management (Sample).xlsx
+++ b/CSci 136 - 05 Test Case Management (Sample).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\OneDrive\Documents\VSU\DCST\BS Computer Science\3rd Year_2024-2025\2nd Semester\CSci 136_Software Engineering 2\Laboratory\LAB 8\MachuPicchuTCM-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CE1CE5-F4E8-4692-943C-985CD677A323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB17A41-F7B8-46CF-86B3-DED62B84FDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="625">
   <si>
     <t>Test Cases</t>
   </si>
@@ -1781,18 +1781,12 @@
     <t xml:space="preserve">  Supplier testing - Delete</t>
   </si>
   <si>
-    <t xml:space="preserve">  Supplier testing - Hide/Show</t>
-  </si>
-  <si>
     <t xml:space="preserve">  Supplier testing - Filter</t>
   </si>
   <si>
     <t xml:space="preserve">  Supplier testing - Search</t>
   </si>
   <si>
-    <t xml:space="preserve">  Supplier testing - Sort</t>
-  </si>
-  <si>
     <t>Verify that supplier is saved and displayed successfully.</t>
   </si>
   <si>
@@ -1802,9 +1796,6 @@
     <t>Verify that supplier is deleted successfully.</t>
   </si>
   <si>
-    <t>Verify that supplier hide/show feature is working successfully.</t>
-  </si>
-  <si>
     <t>SUP-0001</t>
   </si>
   <si>
@@ -1820,12 +1811,6 @@
     <t>SUP-0005</t>
   </si>
   <si>
-    <t>SUP-0006</t>
-  </si>
-  <si>
-    <t>SUP-0007</t>
-  </si>
-  <si>
     <t>Audit Testing</t>
   </si>
   <si>
@@ -1899,6 +1884,18 @@
   </si>
   <si>
     <t xml:space="preserve">Verify that user can log-in successfully. </t>
+  </si>
+  <si>
+    <t>Verify that selecting categories from the filter only shows corresponding products and hides unselected ones..</t>
+  </si>
+  <si>
+    <t>Verify that the category search feature in the "Edit Category" form works successfully.</t>
+  </si>
+  <si>
+    <t>Verify that selecting suppliers from the filter only shows corresponding products and hides unselected ones..</t>
+  </si>
+  <si>
+    <t>Verify that the supplier search feature in the "Edit Supplier" form works successfully.</t>
   </si>
 </sst>
 </file>
@@ -2298,17 +2295,17 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="44.88671875" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.77734375" customWidth="1"/>
+    <col min="3" max="3" width="91.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2325,20 +2322,20 @@
     </row>
     <row r="2" spans="1:3" ht="13.2">
       <c r="A2" s="2" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" s="20" customFormat="1" ht="13.2">
       <c r="A3" s="21" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.2">
@@ -2467,61 +2464,61 @@
     </row>
     <row r="16" spans="1:3" ht="13.2">
       <c r="A16" s="4" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>45</v>
+        <v>621</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="13.2">
       <c r="A17" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>26</v>
+        <v>622</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="13.2">
-      <c r="A18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="A18" s="15" t="s">
+        <v>582</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3" ht="13.2">
       <c r="A19" s="4" t="s">
-        <v>50</v>
+        <v>583</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>51</v>
+        <v>591</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>32</v>
+        <v>588</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="13.2">
-      <c r="A20" s="15" t="s">
-        <v>582</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>592</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="13.2">
       <c r="A21" s="4" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>590</v>
@@ -2529,381 +2526,381 @@
     </row>
     <row r="22" spans="1:3" ht="13.2">
       <c r="A22" s="4" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>591</v>
+        <v>623</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="13.2">
       <c r="A23" s="4" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>592</v>
+        <v>624</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="13.2">
-      <c r="A24" s="4" t="s">
-        <v>586</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>597</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>593</v>
-      </c>
+      <c r="A24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" ht="13.2">
       <c r="A25" s="4" t="s">
-        <v>587</v>
+        <v>53</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>598</v>
+        <v>54</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="13.2">
       <c r="A26" s="4" t="s">
-        <v>588</v>
+        <v>56</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>599</v>
+        <v>57</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="13.2">
       <c r="A27" s="4" t="s">
-        <v>589</v>
+        <v>59</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>600</v>
+        <v>60</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="13.2">
-      <c r="A28" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="A28" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="13.2">
       <c r="A29" s="4" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="13.2">
       <c r="A30" s="4" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="13.2">
       <c r="A31" s="4" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="13.2">
-      <c r="A32" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>64</v>
-      </c>
+      <c r="A32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:3" ht="13.2">
       <c r="A33" s="4" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="13.2">
       <c r="A34" s="4" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>29</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="13.2">
       <c r="A35" s="4" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="13.2">
-      <c r="A36" s="2" t="s">
-        <v>71</v>
+      <c r="A36" s="15" t="s">
+        <v>596</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
     </row>
     <row r="37" spans="1:3" ht="13.2">
-      <c r="A37" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>73</v>
+      <c r="A37" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>601</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="13.2">
-      <c r="A38" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="A38" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" ht="13.2">
       <c r="A39" s="4" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="13.2">
-      <c r="A40" s="15" t="s">
-        <v>601</v>
-      </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="18.600000000000001" customHeight="1">
+      <c r="A40" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="13.2">
-      <c r="A41" s="14" t="s">
-        <v>602</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>606</v>
+      <c r="A41" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="13.2">
       <c r="A42" s="2" t="s">
-        <v>568</v>
+        <v>212</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" ht="13.2">
-      <c r="A43" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="18.600000000000001" customHeight="1">
-      <c r="A44" s="4" t="s">
-        <v>102</v>
+      <c r="A43" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="9"/>
+    </row>
+    <row r="44" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A44" s="14" t="s">
+        <v>614</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>29</v>
+        <v>215</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="13.2">
       <c r="A45" s="4" t="s">
-        <v>104</v>
+        <v>214</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>95</v>
+        <v>228</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="13.2">
-      <c r="A46" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
+      <c r="A46" s="14" t="s">
+        <v>598</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>599</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="13.2">
-      <c r="A47" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="9"/>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A48" s="14" t="s">
-        <v>619</v>
+      <c r="A47" s="14" t="s">
+        <v>600</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="13.2">
+      <c r="A48" s="4" t="s">
+        <v>219</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="C48" s="16" t="s">
-        <v>621</v>
+        <v>602</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="13.2">
       <c r="A49" s="4" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>228</v>
+        <v>603</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="13.2">
-      <c r="A50" s="14" t="s">
-        <v>603</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" customHeight="1">
+      <c r="A50" s="4" t="s">
+        <v>610</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="C50" s="16" t="s">
         <v>604</v>
       </c>
+      <c r="C50" s="6" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="51" spans="1:3" ht="13.2">
-      <c r="A51" s="14" t="s">
-        <v>605</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>566</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>80</v>
-      </c>
+      <c r="A51" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="9"/>
     </row>
     <row r="52" spans="1:3" ht="13.2">
       <c r="A52" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>607</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>220</v>
+        <v>565</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>615</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>605</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="13.2">
-      <c r="A53" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>608</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1">
-      <c r="A54" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>609</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>224</v>
-      </c>
+      <c r="A53" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" ht="13.2">
+      <c r="A54" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="9"/>
     </row>
     <row r="55" spans="1:3" ht="13.2">
-      <c r="A55" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="9"/>
+      <c r="A55" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="56" spans="1:3" ht="13.2">
-      <c r="A56" s="4" t="s">
-        <v>565</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>620</v>
-      </c>
-      <c r="C56" s="16" t="s">
-        <v>610</v>
+      <c r="A56" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="13.2">
-      <c r="A57" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
+      <c r="A57" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="58" spans="1:3" ht="13.2">
-      <c r="A58" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="B58" s="8"/>
-      <c r="C58" s="9"/>
+      <c r="A58" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="59" spans="1:3" ht="13.2">
-      <c r="A59" s="4" t="s">
-        <v>321</v>
+      <c r="A59" s="18" t="s">
+        <v>330</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>323</v>
@@ -2911,10 +2908,10 @@
     </row>
     <row r="60" spans="1:3" ht="13.2">
       <c r="A60" s="18" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>323</v>
@@ -2922,94 +2919,94 @@
     </row>
     <row r="61" spans="1:3" ht="13.2">
       <c r="A61" s="18" t="s">
-        <v>326</v>
+        <v>570</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="13.2">
-      <c r="A62" s="18" t="s">
-        <v>328</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>329</v>
+      <c r="A62" s="19" t="s">
+        <v>609</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>337</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="13.2">
-      <c r="A63" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>331</v>
+      <c r="A63" s="19" t="s">
+        <v>608</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>339</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="13.2">
-      <c r="A64" s="18" t="s">
-        <v>332</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>333</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>323</v>
-      </c>
+      <c r="A64" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B64" s="8"/>
+      <c r="C64" s="9"/>
     </row>
     <row r="65" spans="1:3" ht="13.2">
-      <c r="A65" s="18" t="s">
-        <v>570</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>335</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>323</v>
+      <c r="A65" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="13.2">
-      <c r="A66" s="19" t="s">
-        <v>614</v>
+      <c r="A66" s="18" t="s">
+        <v>324</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>337</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>323</v>
+        <v>343</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="13.2">
-      <c r="A67" s="19" t="s">
-        <v>613</v>
+      <c r="A67" s="18" t="s">
+        <v>326</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>323</v>
+        <v>345</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="13.2">
-      <c r="A68" s="7" t="s">
-        <v>348</v>
-      </c>
-      <c r="B68" s="8"/>
-      <c r="C68" s="9"/>
+      <c r="A68" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="69" spans="1:3" ht="13.2">
-      <c r="A69" s="4" t="s">
-        <v>321</v>
+      <c r="A69" s="18" t="s">
+        <v>330</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>350</v>
@@ -3017,10 +3014,10 @@
     </row>
     <row r="70" spans="1:3" ht="13.2">
       <c r="A70" s="18" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="B70" s="17" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="C70" s="18" t="s">
         <v>350</v>
@@ -3028,359 +3025,359 @@
     </row>
     <row r="71" spans="1:3" ht="13.2">
       <c r="A71" s="18" t="s">
-        <v>326</v>
+        <v>570</v>
       </c>
       <c r="B71" s="17" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="C71" s="18" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="13.2">
-      <c r="A72" s="18" t="s">
-        <v>328</v>
+      <c r="A72" s="19" t="s">
+        <v>609</v>
       </c>
       <c r="B72" s="17" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="13.2">
-      <c r="A73" s="18" t="s">
-        <v>330</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>350</v>
-      </c>
+      <c r="A73" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="B73" s="8"/>
+      <c r="C73" s="9"/>
     </row>
     <row r="74" spans="1:3" ht="13.2">
       <c r="A74" s="18" t="s">
-        <v>332</v>
+        <v>367</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="13.2">
       <c r="A75" s="18" t="s">
-        <v>570</v>
+        <v>373</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="13.2">
-      <c r="A76" s="19" t="s">
-        <v>614</v>
+      <c r="A76" s="18" t="s">
+        <v>376</v>
       </c>
       <c r="B76" s="17" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>350</v>
+        <v>378</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="13.2">
       <c r="A77" s="7" t="s">
-        <v>363</v>
+        <v>382</v>
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="9"/>
     </row>
     <row r="78" spans="1:3" ht="13.2">
       <c r="A78" s="18" t="s">
-        <v>367</v>
+        <v>383</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>369</v>
+        <v>385</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="13.2">
       <c r="A79" s="18" t="s">
-        <v>373</v>
+        <v>386</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="C79" s="18" t="s">
-        <v>375</v>
+        <v>388</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="13.2">
       <c r="A80" s="18" t="s">
-        <v>376</v>
+        <v>389</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="C80" s="18" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="13.2">
-      <c r="A81" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="B81" s="8"/>
-      <c r="C81" s="9"/>
+      <c r="A81" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
     </row>
     <row r="82" spans="1:3" ht="13.2">
-      <c r="A82" s="18" t="s">
-        <v>383</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="C82" s="18" t="s">
-        <v>385</v>
-      </c>
+      <c r="A82" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="B82" s="8"/>
+      <c r="C82" s="9"/>
     </row>
     <row r="83" spans="1:3" ht="13.2">
-      <c r="A83" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="B83" s="17" t="s">
-        <v>358</v>
-      </c>
-      <c r="C83" s="18" t="s">
-        <v>388</v>
+      <c r="A83" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="13.2">
-      <c r="A84" s="18" t="s">
-        <v>389</v>
-      </c>
-      <c r="B84" s="17" t="s">
-        <v>359</v>
-      </c>
-      <c r="C84" s="18" t="s">
-        <v>391</v>
+      <c r="A84" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="13.2">
-      <c r="A85" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
+      <c r="A85" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="13.2">
-      <c r="A86" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="B86" s="8"/>
-      <c r="C86" s="9"/>
+      <c r="A86" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="87" spans="1:3" ht="13.2">
       <c r="A87" s="4" t="s">
-        <v>394</v>
+        <v>406</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="13.2">
-      <c r="A88" s="4" t="s">
-        <v>397</v>
+      <c r="A88" s="14" t="s">
+        <v>409</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>398</v>
+        <v>410</v>
       </c>
       <c r="C88" s="12" t="s">
-        <v>399</v>
+        <v>411</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="13.2">
-      <c r="A89" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="C89" s="12" t="s">
-        <v>402</v>
-      </c>
+      <c r="A89" s="13" t="s">
+        <v>571</v>
+      </c>
+      <c r="B89" s="8"/>
+      <c r="C89" s="9"/>
     </row>
     <row r="90" spans="1:3" ht="13.2">
       <c r="A90" s="4" t="s">
-        <v>616</v>
+        <v>572</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="C90" s="12" t="s">
-        <v>405</v>
+        <v>576</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="13.2">
       <c r="A91" s="4" t="s">
-        <v>406</v>
+        <v>573</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>408</v>
+        <v>577</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="13.2">
-      <c r="A92" s="14" t="s">
-        <v>409</v>
+      <c r="A92" s="4" t="s">
+        <v>574</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>410</v>
+        <v>422</v>
       </c>
       <c r="C92" s="12" t="s">
-        <v>411</v>
+        <v>578</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="13.2">
-      <c r="A93" s="13" t="s">
-        <v>571</v>
-      </c>
-      <c r="B93" s="8"/>
-      <c r="C93" s="9"/>
+      <c r="A93" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="94" spans="1:3" ht="13.2">
       <c r="A94" s="4" t="s">
-        <v>572</v>
+        <v>581</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>416</v>
+        <v>428</v>
       </c>
       <c r="C94" s="12" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="13.2">
-      <c r="A95" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="C95" s="12" t="s">
-        <v>577</v>
-      </c>
+      <c r="A95" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
     </row>
     <row r="96" spans="1:3" ht="13.2">
-      <c r="A96" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="C96" s="12" t="s">
-        <v>578</v>
-      </c>
+      <c r="A96" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="B96" s="8"/>
+      <c r="C96" s="9"/>
     </row>
     <row r="97" spans="1:3" ht="13.2">
       <c r="A97" s="4" t="s">
-        <v>575</v>
+        <v>612</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>425</v>
-      </c>
-      <c r="C97" s="12" t="s">
-        <v>579</v>
+        <v>433</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="13.2">
-      <c r="A98" s="4" t="s">
-        <v>581</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="C98" s="12" t="s">
-        <v>580</v>
-      </c>
+      <c r="A98" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="B98" s="8"/>
+      <c r="C98" s="9"/>
     </row>
     <row r="99" spans="1:3" ht="13.2">
-      <c r="A99" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
+      <c r="A99" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="B99" s="8"/>
+      <c r="C99" s="9"/>
     </row>
     <row r="100" spans="1:3" ht="13.2">
-      <c r="A100" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="B100" s="8"/>
-      <c r="C100" s="9"/>
+      <c r="A100" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B100" s="17" t="s">
+        <v>436</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="101" spans="1:3" ht="13.2">
-      <c r="A101" s="4" t="s">
-        <v>617</v>
-      </c>
-      <c r="B101" s="5" t="s">
-        <v>433</v>
+      <c r="A101" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="B101" s="17" t="s">
+        <v>439</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>437</v>
+        <v>466</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="13.2">
-      <c r="A102" s="7" t="s">
-        <v>462</v>
-      </c>
-      <c r="B102" s="8"/>
-      <c r="C102" s="9"/>
+      <c r="A102" s="18" t="s">
+        <v>469</v>
+      </c>
+      <c r="B102" s="17" t="s">
+        <v>442</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="103" spans="1:3" ht="13.2">
-      <c r="A103" s="7" t="s">
-        <v>463</v>
-      </c>
-      <c r="B103" s="8"/>
-      <c r="C103" s="9"/>
+      <c r="A103" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="B103" s="17" t="s">
+        <v>445</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="104" spans="1:3" ht="13.2">
-      <c r="A104" s="4" t="s">
-        <v>464</v>
+      <c r="A104" s="18" t="s">
+        <v>473</v>
       </c>
       <c r="B104" s="17" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="13.2">
-      <c r="A105" s="18" t="s">
-        <v>467</v>
+      <c r="A105" s="19" t="s">
+        <v>606</v>
       </c>
       <c r="B105" s="17" t="s">
-        <v>439</v>
+        <v>451</v>
       </c>
       <c r="C105" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="13.2">
-      <c r="A106" s="18" t="s">
-        <v>469</v>
+      <c r="A106" s="19" t="s">
+        <v>607</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>442</v>
+        <v>454</v>
       </c>
       <c r="C106" s="6" t="s">
         <v>466</v>
@@ -3388,94 +3385,94 @@
     </row>
     <row r="107" spans="1:3" ht="13.2">
       <c r="A107" s="18" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="B107" s="17" t="s">
-        <v>445</v>
+        <v>457</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="13.2">
-      <c r="A108" s="18" t="s">
-        <v>473</v>
-      </c>
-      <c r="B108" s="17" t="s">
-        <v>448</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>466</v>
-      </c>
+      <c r="A108" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="B108" s="8"/>
+      <c r="C108" s="9"/>
     </row>
     <row r="109" spans="1:3" ht="13.2">
-      <c r="A109" s="19" t="s">
-        <v>611</v>
+      <c r="A109" s="4" t="s">
+        <v>464</v>
       </c>
       <c r="B109" s="17" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="C109" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="13.2">
-      <c r="A110" s="19" t="s">
-        <v>612</v>
+      <c r="A110" s="4" t="s">
+        <v>613</v>
       </c>
       <c r="B110" s="17" t="s">
-        <v>454</v>
+        <v>465</v>
       </c>
       <c r="C110" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="13.2">
-      <c r="A111" s="18" t="s">
-        <v>475</v>
+      <c r="A111" s="4" t="s">
+        <v>469</v>
       </c>
       <c r="B111" s="17" t="s">
-        <v>457</v>
+        <v>468</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="13.2">
-      <c r="A112" s="7" t="s">
-        <v>489</v>
-      </c>
-      <c r="B112" s="8"/>
-      <c r="C112" s="9"/>
+      <c r="A112" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="B112" s="17" t="s">
+        <v>470</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="113" spans="1:3" ht="13.2">
       <c r="A113" s="4" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="B113" s="17" t="s">
-        <v>460</v>
+        <v>472</v>
       </c>
       <c r="C113" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="13.2">
-      <c r="A114" s="4" t="s">
-        <v>618</v>
+      <c r="A114" s="19" t="s">
+        <v>606</v>
       </c>
       <c r="B114" s="17" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="C114" s="6" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="13.2">
-      <c r="A115" s="4" t="s">
-        <v>469</v>
+      <c r="A115" s="19" t="s">
+        <v>607</v>
       </c>
       <c r="B115" s="17" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="C115" s="6" t="s">
         <v>466</v>
@@ -3483,10 +3480,10 @@
     </row>
     <row r="116" spans="1:3" ht="13.2">
       <c r="A116" s="4" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="B116" s="17" t="s">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="C116" s="6" t="s">
         <v>466</v>
@@ -3494,96 +3491,52 @@
     </row>
     <row r="117" spans="1:3" ht="13.2">
       <c r="A117" s="4" t="s">
-        <v>473</v>
+        <v>502</v>
       </c>
       <c r="B117" s="17" t="s">
-        <v>472</v>
+        <v>480</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>466</v>
+        <v>504</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="13.2">
-      <c r="A118" s="19" t="s">
-        <v>611</v>
-      </c>
-      <c r="B118" s="17" t="s">
-        <v>474</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>466</v>
-      </c>
+      <c r="A118" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
     </row>
     <row r="119" spans="1:3" ht="13.2">
-      <c r="A119" s="19" t="s">
-        <v>612</v>
-      </c>
-      <c r="B119" s="17" t="s">
-        <v>476</v>
+      <c r="A119" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>510</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>466</v>
+        <v>520</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="13.2">
       <c r="A120" s="4" t="s">
-        <v>475</v>
-      </c>
-      <c r="B120" s="17" t="s">
-        <v>478</v>
+        <v>521</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>513</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>466</v>
+        <v>523</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="13.2">
       <c r="A121" s="4" t="s">
-        <v>502</v>
-      </c>
-      <c r="B121" s="17" t="s">
-        <v>480</v>
+        <v>524</v>
+      </c>
+      <c r="B121" s="5" t="s">
+        <v>516</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="13.2">
-      <c r="A122" s="2" t="s">
-        <v>505</v>
-      </c>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-    </row>
-    <row r="123" spans="1:3" ht="13.2">
-      <c r="A123" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="13.2">
-      <c r="A124" s="4" t="s">
-        <v>521</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="13.2">
-      <c r="A125" s="4" t="s">
-        <v>524</v>
-      </c>
-      <c r="B125" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="C125" s="6" t="s">
         <v>526</v>
       </c>
     </row>

</xml_diff>